<commit_message>
test changes in b6607bb
</commit_message>
<xml_diff>
--- a/run/output/iecorrect/hyphen-id.xlsx
+++ b/run/output/iecorrect/hyphen-id.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,19 +10,19 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0372F159-AAC6-4802-9601-ACFABBA81058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27645" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27645" windowHeight="16440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="string" sheetId="1" r:id="rId1"/>
     <sheet name="numeric" sheetId="2" r:id="rId2"/>
     <sheet name="drop" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="62" uniqueCount="15">
   <si>
     <t>make</t>
   </si>
@@ -52,12 +52,27 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>n_changes</t>
+  </si>
+  <si>
+    <t>date_last_changed</t>
+  </si>
+  <si>
+    <t>11 Dec 2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -93,7 +108,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -112,7 +127,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -263,7 +278,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -287,9 +302,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -313,7 +328,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -348,7 +363,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -366,7 +381,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -391,7 +406,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -407,7 +422,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -416,7 +431,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,7 +451,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2">
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -447,16 +462,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -475,22 +490,38 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
+    <row r="2">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -498,14 +529,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -519,7 +550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>

</xml_diff>